<commit_message>
3tp haste calculation adjusted
</commit_message>
<xml_diff>
--- a/functionality.xlsx
+++ b/functionality.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Rotation support (haste)</t>
   </si>
@@ -67,6 +67,24 @@
   </si>
   <si>
     <t>Filter out nonusable items</t>
+  </si>
+  <si>
+    <t>Grab itemID/link from mouseover</t>
+  </si>
+  <si>
+    <t>Grab IitemID/link from mouseover comparison(shift)</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>todo</t>
+  </si>
+  <si>
+    <t>OsF 3tp support</t>
+  </si>
+  <si>
+    <t>proper rotation support</t>
   </si>
 </sst>
 </file>
@@ -123,9 +141,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G21"/>
+  <dimension ref="B2:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,6 +481,9 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
       <c r="F3" t="s">
         <v>0</v>
       </c>
@@ -468,6 +492,9 @@
       <c r="B4" t="s">
         <v>9</v>
       </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
       <c r="F4" t="s">
         <v>1</v>
       </c>
@@ -476,6 +503,9 @@
       <c r="B5" t="s">
         <v>10</v>
       </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
       <c r="F5" t="s">
         <v>2</v>
       </c>
@@ -484,6 +514,9 @@
       <c r="B6" t="s">
         <v>11</v>
       </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
       <c r="F6" t="s">
         <v>3</v>
       </c>
@@ -492,35 +525,71 @@
       <c r="B7" t="s">
         <v>15</v>
       </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
       <c r="F7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="2">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>